<commit_message>
Góp ý lần 1
Góp ý lần 1
</commit_message>
<xml_diff>
--- a/QuanLySuCo_2018_11_08/3-Coding/code/DesktopModules/QLSC/bieumau/BAO_CAO_THANG.xlsx
+++ b/QuanLySuCo_2018_11_08/3-Coding/code/DesktopModules/QLSC/bieumau/BAO_CAO_THANG.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <r>
       <t>CỘNG TY ĐIỆN LỰC SÓC TRĂNG</t>
@@ -174,12 +174,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tình hình sự cố tháng từ ngày 01 đến ngày 28/02/2018   </t>
-  </si>
-  <si>
-    <t>hhh</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
 </sst>
 </file>
@@ -404,7 +398,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -561,66 +555,78 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="20" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1221,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="16.5"/>
@@ -1232,7 +1238,7 @@
     <col min="3" max="4" width="5.85546875" style="38" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="4" customWidth="1"/>
     <col min="8" max="8" width="6" style="4" customWidth="1"/>
     <col min="9" max="9" width="5.5703125" style="62" customWidth="1"/>
     <col min="10" max="10" width="4.42578125" style="4" customWidth="1"/>
@@ -2774,7 +2780,7 @@
       <c r="D1" s="76"/>
       <c r="E1" s="76"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="65"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -2851,7 +2857,7 @@
       <c r="D4" s="74"/>
       <c r="E4" s="74"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="G4" s="64"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -2872,58 +2878,58 @@
       <c r="W4" s="75"/>
     </row>
     <row r="5" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="65"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="65"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
     </row>
     <row r="6" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="65"/>
-      <c r="U6" s="65"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="65"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+      <c r="S6" s="70"/>
+      <c r="T6" s="70"/>
+      <c r="U6" s="70"/>
+      <c r="V6" s="70"/>
+      <c r="W6" s="70"/>
     </row>
     <row r="7" spans="1:256" ht="18.75">
       <c r="A7" s="7"/>
@@ -2932,7 +2938,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="G7" s="66"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -2951,57 +2957,57 @@
       <c r="W7" s="7"/>
     </row>
     <row r="8" spans="1:256">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="72" t="s">
+      <c r="E8" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="72" t="s">
+      <c r="F8" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="72" t="s">
+      <c r="G8" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="72" t="s">
+      <c r="H8" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72" t="s">
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="72" t="s">
+      <c r="L8" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="72" t="s">
+      <c r="M8" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="72" t="s">
+      <c r="N8" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="72"/>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
-      <c r="R8" s="72"/>
-      <c r="S8" s="72"/>
-      <c r="T8" s="73" t="s">
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="73"/>
+      <c r="S8" s="73"/>
+      <c r="T8" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="U8" s="72" t="s">
+      <c r="U8" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="V8" s="72"/>
-      <c r="W8" s="72" t="s">
+      <c r="V8" s="73"/>
+      <c r="W8" s="73" t="s">
         <v>18</v>
       </c>
       <c r="X8" s="8"/>
@@ -3239,62 +3245,62 @@
       <c r="IV8" s="8"/>
     </row>
     <row r="9" spans="1:256" s="9" customFormat="1">
-      <c r="A9" s="80"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72" t="s">
+      <c r="A9" s="71"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="72" t="s">
+      <c r="I9" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="72" t="s">
+      <c r="J9" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="72" t="s">
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="72"/>
-      <c r="P9" s="72" t="s">
+      <c r="O9" s="73"/>
+      <c r="P9" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="Q9" s="72"/>
-      <c r="R9" s="72" t="s">
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="S9" s="72" t="s">
+      <c r="S9" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="T9" s="73"/>
-      <c r="U9" s="72" t="s">
+      <c r="T9" s="86"/>
+      <c r="U9" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="V9" s="72" t="s">
+      <c r="V9" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="W9" s="72"/>
+      <c r="W9" s="73"/>
     </row>
     <row r="10" spans="1:256" s="9" customFormat="1" ht="36">
-      <c r="A10" s="80"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="72"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
       <c r="N10" s="10" t="s">
         <v>28</v>
       </c>
@@ -3307,12 +3313,12 @@
       <c r="Q10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R10" s="72"/>
-      <c r="S10" s="72"/>
-      <c r="T10" s="73"/>
-      <c r="U10" s="72"/>
-      <c r="V10" s="72"/>
-      <c r="W10" s="72"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="73"/>
+      <c r="T10" s="86"/>
+      <c r="U10" s="73"/>
+      <c r="V10" s="73"/>
+      <c r="W10" s="73"/>
     </row>
     <row r="11" spans="1:256" s="48" customFormat="1" ht="12.75">
       <c r="A11" s="44"/>
@@ -3323,82 +3329,48 @@
         <v>30</v>
       </c>
       <c r="F11" s="47"/>
-      <c r="G11" s="82" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="58">
-        <v>1</v>
-      </c>
-      <c r="J11" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="M11" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="N11" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="O11" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q11" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="R11" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="S11" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="T11" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="U11" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="V11" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="W11" s="50" t="s">
-        <v>40</v>
-      </c>
+      <c r="G11" s="68"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="50"/>
+      <c r="T11" s="51"/>
+      <c r="U11" s="50"/>
+      <c r="V11" s="50"/>
+      <c r="W11" s="50"/>
     </row>
     <row r="12" spans="1:256">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="67"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="53"/>
       <c r="D12" s="53"/>
       <c r="E12" s="2"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="53"/>
       <c r="H12" s="2"/>
       <c r="I12" s="59"/>
       <c r="J12" s="2"/>
-      <c r="O12" s="68" t="s">
+      <c r="O12" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="68"/>
-      <c r="R12" s="68"/>
-      <c r="S12" s="68"/>
-      <c r="T12" s="68"/>
-      <c r="U12" s="68"/>
-      <c r="V12" s="68"/>
-      <c r="W12" s="68"/>
+      <c r="P12" s="82"/>
+      <c r="Q12" s="82"/>
+      <c r="R12" s="82"/>
+      <c r="S12" s="82"/>
+      <c r="T12" s="82"/>
+      <c r="U12" s="82"/>
+      <c r="V12" s="82"/>
+      <c r="W12" s="82"/>
     </row>
     <row r="13" spans="1:256" s="17" customFormat="1" ht="12">
       <c r="A13" s="12" t="s">
@@ -3409,7 +3381,7 @@
       <c r="D13" s="54"/>
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="14"/>
+      <c r="G13" s="54"/>
       <c r="H13" s="14"/>
       <c r="I13" s="60"/>
       <c r="J13" s="14"/>
@@ -3419,12 +3391,12 @@
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="16"/>
-      <c r="Q13" s="69"/>
-      <c r="R13" s="69"/>
-      <c r="S13" s="69"/>
-      <c r="T13" s="69"/>
-      <c r="U13" s="69"/>
-      <c r="V13" s="69"/>
+      <c r="Q13" s="83"/>
+      <c r="R13" s="83"/>
+      <c r="S13" s="83"/>
+      <c r="T13" s="83"/>
+      <c r="U13" s="83"/>
+      <c r="V13" s="83"/>
       <c r="W13" s="14"/>
       <c r="X13" s="14"/>
       <c r="Y13" s="14"/>
@@ -3641,7 +3613,7 @@
       <c r="D14" s="54"/>
       <c r="E14" s="14"/>
       <c r="F14" s="18"/>
-      <c r="G14" s="14"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="14"/>
       <c r="I14" s="60"/>
       <c r="J14" s="14"/>
@@ -3873,7 +3845,7 @@
       <c r="D15" s="54"/>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="14"/>
+      <c r="G15" s="54"/>
       <c r="H15" s="14"/>
       <c r="I15" s="60"/>
       <c r="J15" s="14"/>
@@ -4103,7 +4075,7 @@
       <c r="D16" s="55"/>
       <c r="E16" s="22"/>
       <c r="F16" s="23"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="53"/>
       <c r="H16" s="2"/>
       <c r="I16" s="59"/>
       <c r="J16" s="2"/>
@@ -4117,16 +4089,16 @@
       <c r="D17" s="56"/>
       <c r="E17" s="26"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="G17" s="53"/>
       <c r="H17" s="2"/>
       <c r="I17" s="59"/>
       <c r="J17" s="2"/>
       <c r="P17" s="24"/>
-      <c r="Q17" s="70"/>
-      <c r="R17" s="70"/>
-      <c r="S17" s="70"/>
-      <c r="T17" s="70"/>
-      <c r="U17" s="70"/>
+      <c r="Q17" s="84"/>
+      <c r="R17" s="84"/>
+      <c r="S17" s="84"/>
+      <c r="T17" s="84"/>
+      <c r="U17" s="84"/>
       <c r="W17" s="27"/>
     </row>
     <row r="18" spans="1:256">
@@ -4136,7 +4108,7 @@
       <c r="D18" s="56"/>
       <c r="E18" s="26"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="53"/>
       <c r="H18" s="2"/>
       <c r="I18" s="59"/>
       <c r="J18" s="2"/>
@@ -4382,7 +4354,7 @@
       <c r="D19" s="40"/>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
-      <c r="G19" s="32"/>
+      <c r="G19" s="67"/>
       <c r="H19" s="32"/>
       <c r="I19" s="61"/>
       <c r="J19" s="32"/>
@@ -4426,17 +4398,17 @@
       <c r="D20" s="40"/>
       <c r="E20" s="31"/>
       <c r="F20" s="35"/>
-      <c r="G20" s="32"/>
+      <c r="G20" s="67"/>
       <c r="H20" s="32"/>
       <c r="I20" s="61"/>
       <c r="J20" s="32"/>
-      <c r="Q20" s="68"/>
-      <c r="R20" s="68"/>
-      <c r="S20" s="68"/>
-      <c r="T20" s="68"/>
-      <c r="U20" s="68"/>
-      <c r="V20" s="68"/>
-      <c r="W20" s="68"/>
+      <c r="Q20" s="82"/>
+      <c r="R20" s="82"/>
+      <c r="S20" s="82"/>
+      <c r="T20" s="82"/>
+      <c r="U20" s="82"/>
+      <c r="V20" s="82"/>
+      <c r="W20" s="82"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
@@ -4939,8 +4911,8 @@
       <c r="C25" s="38"/>
       <c r="D25" s="30"/>
       <c r="E25" s="32"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
       <c r="H25" s="43"/>
       <c r="I25" s="63"/>
       <c r="J25" s="43"/>
@@ -5180,36 +5152,14 @@
     </row>
     <row r="26" spans="1:256" ht="18.75">
       <c r="A26" s="29"/>
-      <c r="P26" s="66"/>
-      <c r="Q26" s="66"/>
-      <c r="R26" s="66"/>
-      <c r="S26" s="66"/>
+      <c r="P26" s="80"/>
+      <c r="Q26" s="80"/>
+      <c r="R26" s="80"/>
+      <c r="S26" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A5:W5"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="M4:W4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="A3:W3"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="W8:W10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="N9:O9"/>
     <mergeCell ref="P9:Q9"/>
     <mergeCell ref="A6:W6"/>
     <mergeCell ref="P26:S26"/>
@@ -5226,7 +5176,29 @@
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
-    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="M4:W4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="A3:W3"/>
+    <mergeCell ref="A5:W5"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="W8:W10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="R9:R10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>